<commit_message>
Lista de componentes casi actualizada
</commit_message>
<xml_diff>
--- a/PCB_Design/Lista_componentes.xlsx
+++ b/PCB_Design/Lista_componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegofigueroa/Documents/GitHub/RemoteTempMonitor/PCB_Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A112C3-EEAD-EC49-94E0-A26B894F08AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B23F8B-14C8-7C4E-9492-FCD8D794CC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{06313240-559F-D04A-8DD7-FFF8CB69C591}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="PCB_Design" localSheetId="0">Hoja1!$A$1:$D$32</definedName>
+    <definedName name="PCB_Design" localSheetId="0">Hoja1!$A$1:$D$31</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,9 +67,6 @@
     <t>4.7k1</t>
   </si>
   <si>
-    <t>R_OneWire</t>
-  </si>
-  <si>
     <t>Battery_Cell</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>10u</t>
   </si>
   <si>
-    <t>1u</t>
-  </si>
-  <si>
     <t>Conn_I2C1</t>
   </si>
   <si>
@@ -133,24 +127,12 @@
     <t>R1</t>
   </si>
   <si>
-    <t>1M</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>590k</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
-    <t>R_PROG1</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>R_rLed1</t>
   </si>
   <si>
@@ -214,9 +196,6 @@
     <t>Sigma</t>
   </si>
   <si>
-    <t>USB-C</t>
-  </si>
-  <si>
     <t>Mactrónica</t>
   </si>
   <si>
@@ -226,9 +205,6 @@
     <t>Mercado Libre</t>
   </si>
   <si>
-    <t>Ferretrónica</t>
-  </si>
-  <si>
     <t>NMOS</t>
   </si>
   <si>
@@ -269,13 +245,37 @@
   </si>
   <si>
     <t>Danny</t>
+  </si>
+  <si>
+    <t>USB-b micro</t>
+  </si>
+  <si>
+    <t>cantidad compra</t>
+  </si>
+  <si>
+    <t>Centro</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>centro</t>
+  </si>
+  <si>
+    <t>6.98k</t>
+  </si>
+  <si>
+    <t>4.02k</t>
+  </si>
+  <si>
+    <t>R_OneWire R_PROG1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,8 +290,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +323,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -329,13 +354,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A532B50-098F-2142-9F42-C1BD222C66BC}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,10 +697,12 @@
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -685,47 +716,50 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="I2">
+        <v>47</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="J2">
         <f>G2*B2</f>
         <v>0</v>
       </c>
-      <c r="K2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -733,34 +767,37 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3">
         <v>5000</v>
       </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I32" si="0">G3*B3</f>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3">
+        <f>G3*H3</f>
         <v>10000</v>
       </c>
-      <c r="K3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3">
-        <f>SUMIF(H2:H32,"Diego",I2:I32)</f>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3">
+        <f>SUMIF(I2:I31,"Diego",J2:J31)</f>
         <v>30000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -768,28 +805,28 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4">
-        <f>SUMIF(H2:H32,"Omar",I2:I32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <f t="shared" ref="J4:J31" si="0">G4*H4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4">
+        <f>SUMIF(I2:I31,"Omar",J2:J31)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -797,28 +834,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5">
-        <f>SUMIF(H2:H32,"Danny",I2:I32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5">
+        <f>SUMIF(I2:I31,"Danny",J2:J31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -826,21 +863,21 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
+      <c r="E6" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -848,21 +885,21 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -870,21 +907,21 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -892,21 +929,21 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -914,21 +951,21 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -936,21 +973,21 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -958,21 +995,21 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -980,27 +1017,30 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13">
         <v>1000</v>
       </c>
-      <c r="H13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1008,21 +1048,21 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1030,21 +1070,21 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1052,21 +1092,21 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1074,21 +1114,30 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17">
+        <v>1000</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1096,21 +1145,21 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1118,21 +1167,21 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1140,21 +1189,21 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1162,21 +1211,21 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1184,250 +1233,240 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D22">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23">
+        <v>47</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24">
+        <v>300</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
         <v>31</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D24">
-        <v>47</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25">
-        <v>270</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="4"/>
-      <c r="G32">
+      <c r="F31" s="4"/>
+      <c r="G31">
         <v>19000</v>
       </c>
-      <c r="H32" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32">
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="0"/>
         <v>19000</v>
       </c>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I33">
-        <f>SUM(I2:I32)</f>
-        <v>30000</v>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <f>SUM(J2:J31)</f>
+        <v>31000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>